<commit_message>
Add bonnie++ results to results.xlsx
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18560" yWindow="1460" windowWidth="28800" windowHeight="27340" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="22400" yWindow="460" windowWidth="28800" windowHeight="21140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CPU" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>OPENSHIFT</t>
   </si>
@@ -58,6 +58,36 @@
   </si>
   <si>
     <t>read</t>
+  </si>
+  <si>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>Block (sequential)</t>
+  </si>
+  <si>
+    <t>Per-Character (stdio and sequential)</t>
+  </si>
+  <si>
+    <t>Per-Character (stdio)</t>
+  </si>
+  <si>
+    <t>Rewrite (cache + IO)</t>
+  </si>
+  <si>
+    <t>Random Seeks - READ and WRITE in /sec</t>
+  </si>
+  <si>
+    <t>Sequential Output - WRITE in Kb/sec</t>
+  </si>
+  <si>
+    <t>Sequential Input - READ in Kb/sec</t>
+  </si>
+  <si>
+    <t>bonnie++</t>
+  </si>
+  <si>
+    <t>monkeytest</t>
   </si>
 </sst>
 </file>
@@ -67,7 +97,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -129,21 +159,67 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -154,7 +230,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -164,6 +240,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -447,7 +537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H64"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A3" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A32" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
@@ -1604,53 +1694,196 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D6"/>
+  <dimension ref="A3:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="11">
+        <v>216</v>
+      </c>
+      <c r="C7" s="11">
+        <v>477</v>
+      </c>
+      <c r="D7" s="11">
+        <v>649</v>
+      </c>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="11">
+        <v>714982</v>
+      </c>
+      <c r="C8" s="11">
+        <v>317874</v>
+      </c>
+      <c r="D8" s="11">
+        <v>77161</v>
+      </c>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="11">
+        <v>771912</v>
+      </c>
+      <c r="C9" s="11">
+        <v>264559</v>
+      </c>
+      <c r="D9" s="11">
+        <v>78075</v>
+      </c>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="11">
+        <v>855</v>
+      </c>
+      <c r="C12" s="11">
+        <v>1429</v>
+      </c>
+      <c r="D12" s="11">
+        <v>1961</v>
+      </c>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="11">
+        <v>3051978</v>
+      </c>
+      <c r="C13" s="11">
+        <v>2157337</v>
+      </c>
+      <c r="D13" s="11">
+        <v>1188254</v>
+      </c>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="11">
+        <v>96</v>
+      </c>
+      <c r="C15" s="11">
+        <v>7395</v>
+      </c>
+      <c r="D15" s="11">
+        <v>6331</v>
+      </c>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="8"/>
+    </row>
+    <row r="20" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B21" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
+      <c r="C21" s="12">
         <v>127.16</v>
       </c>
-      <c r="D5">
+      <c r="D21" s="12">
         <v>34.270000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B22" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C6">
+      <c r="C22" s="12">
         <v>9.73</v>
       </c>
-      <c r="D6">
+      <c r="D22" s="12">
         <v>176.84</v>
       </c>
     </row>

</xml_diff>